<commit_message>
added contact to excel
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CS1039C\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CS1039C\Desktop\git-eny\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
   <si>
     <t>First Name</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Fakhiri</t>
+  </si>
+  <si>
+    <t>Ram</t>
   </si>
 </sst>
 </file>
@@ -545,13 +548,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X39"/>
+  <dimension ref="A1:X40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomRight" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1975,6 +1978,11 @@
         <v>55</v>
       </c>
     </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Y1"/>
   <dataValidations count="1">

</xml_diff>